<commit_message>
QM working. Data getting into Orch queue.
</commit_message>
<xml_diff>
--- a/CustomREFramework_Dispatcher/Data/Config.xlsx
+++ b/CustomREFramework_Dispatcher/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James\Documents\UiPath\custom-rpa-uipath-reframework\CustomREFramework_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E5257F-3F6B-42D5-AAF4-818760600BC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{785DE961-A88A-4071-909F-C8C9BA23DDD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6720" yWindow="1320" windowWidth="21030" windowHeight="13050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="62">
   <si>
     <t>Name</t>
   </si>
@@ -183,7 +183,34 @@
     <t>A1:C</t>
   </si>
   <si>
-    <t>C:\Users\James\Documents\UiPath\custom-rpa-uipath-reframework\CustomREFramework_Dispatcher\Data\DispatchExcel.xlsx</t>
+    <t xml:space="preserve">DeletePriorRunNewQueueItems </t>
+  </si>
+  <si>
+    <t>ApplicationUserNames</t>
+  </si>
+  <si>
+    <t>NextJobProcessName</t>
+  </si>
+  <si>
+    <t>RetryCount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RetryIntervalSeconds </t>
+  </si>
+  <si>
+    <t>StartJobApiJsonBody</t>
+  </si>
+  <si>
+    <t>EnableFaultOnError</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QueueItemReferenceKey </t>
+  </si>
+  <si>
+    <t>Data\DispatchExcel.xlsx</t>
+  </si>
+  <si>
+    <t>Reference</t>
   </si>
 </sst>
 </file>
@@ -566,16 +593,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z997"/>
+  <dimension ref="A1:Z995"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C19:C20"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="43" style="2" customWidth="1"/>
+    <col min="1" max="1" width="31" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="81.42578125" style="2" customWidth="1"/>
     <col min="4" max="26" width="8.7109375" style="2" customWidth="1"/>
     <col min="27" max="16384" width="14.42578125" style="2"/>
@@ -651,7 +678,7 @@
         <v>45</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
@@ -678,14 +705,61 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A16" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
     <row r="19" ht="14.25" customHeight="1"/>
@@ -1665,8 +1739,6 @@
     <row r="993" ht="14.25" customHeight="1"/>
     <row r="994" ht="14.25" customHeight="1"/>
     <row r="995" ht="14.25" customHeight="1"/>
-    <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>